<commit_message>
yargi 2 and 3
</commit_message>
<xml_diff>
--- a/cost.xlsx
+++ b/cost.xlsx
@@ -196,11 +196,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -284,10 +284,10 @@
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.16"/>
@@ -354,7 +354,7 @@
       <c r="B2" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="6" t="n">
         <f aca="false">B2*500</f>
         <v>6000</v>
       </c>
@@ -362,31 +362,31 @@
         <f aca="false">(C2*500)+(D2*500)</f>
         <v>0</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="6" t="n">
         <v>2400</v>
       </c>
-      <c r="H2" s="7" t="n">
+      <c r="H2" s="6" t="n">
         <f aca="false">E2+F2+G2</f>
         <v>8400</v>
       </c>
       <c r="J2" s="0" t="n">
         <f aca="false">SUM(H2:H5)</f>
-        <v>46800</v>
+        <v>49200</v>
       </c>
       <c r="K2" s="0" t="n">
         <f aca="false">J2*0.015</f>
-        <v>702</v>
+        <v>738</v>
       </c>
       <c r="L2" s="0" t="n">
         <f aca="false">J2+K2</f>
-        <v>47502</v>
+        <v>49938</v>
       </c>
       <c r="M2" s="0" t="n">
         <v>70500</v>
       </c>
       <c r="N2" s="0" t="n">
         <f aca="false">M2-L2</f>
-        <v>22998</v>
+        <v>20562</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -406,11 +406,11 @@
         <f aca="false">B3*500</f>
         <v>6000</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="7" t="n">
         <f aca="false">(C3*500)+(D3*500)</f>
         <v>6000</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="6" t="n">
         <v>2400</v>
       </c>
       <c r="H3" s="0" t="n">
@@ -440,14 +440,16 @@
         <f aca="false">B4*500</f>
         <v>7000</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="7" t="n">
         <f aca="false">(C4*500)+(D4*500)</f>
         <v>7000</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="6" t="n">
+        <v>2400</v>
+      </c>
       <c r="H4" s="0" t="n">
         <f aca="false">E4+F4+G4</f>
-        <v>14000</v>
+        <v>16400</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -463,15 +465,15 @@
       <c r="D5" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="7" t="n">
         <f aca="false">B5*500</f>
         <v>5000</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="7" t="n">
         <f aca="false">(C5*500)+(D5*500)</f>
         <v>5000</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="0" t="n">
         <f aca="false">E5+F5+G5</f>
         <v>10000</v>

</xml_diff>

<commit_message>
added the god father
</commit_message>
<xml_diff>
--- a/cost.xlsx
+++ b/cost.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lord of the rings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The god father</t>
   </si>
 </sst>
 </file>
@@ -345,13 +348,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.89"/>
@@ -793,6 +796,28 @@
         <v>3200</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9" t="n">
+        <f aca="false">B13*500</f>
+        <v>8500</v>
+      </c>
+      <c r="I13" s="9" t="n">
+        <f aca="false">B13*200</f>
+        <v>3400</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>